<commit_message>
@Editfeature - added some fields in sheet while uploading society master data through sheet
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/society_data.xlsx
+++ b/coreapi/coreapi/v0/society_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t xml:space="preserve">Society Name</t>
   </si>
@@ -34,12 +34,27 @@
     <t xml:space="preserve">Subarea</t>
   </si>
   <si>
+    <t xml:space="preserve">Society Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supplier Code</t>
   </si>
   <si>
+    <t xml:space="preserve">supplier_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zipcode</t>
   </si>
   <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Society Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Latitude</t>
   </si>
   <si>
@@ -52,6 +67,12 @@
     <t xml:space="preserve">Flat Count</t>
   </si>
   <si>
+    <t xml:space="preserve">No of Vacant flats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelor Tenants allowed?</t>
+  </si>
+  <si>
     <t xml:space="preserve">designation</t>
   </si>
   <si>
@@ -79,6 +100,12 @@
     <t xml:space="preserve">Account No</t>
   </si>
   <si>
+    <t xml:space="preserve">Relationship Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year Of Possetion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stall Allowed(Y/N)</t>
   </si>
   <si>
@@ -118,7 +145,7 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">Jelly Beans</t>
+    <t xml:space="preserve">Jelly Beans test</t>
   </si>
   <si>
     <t xml:space="preserve">BEN</t>
@@ -130,7 +157,25 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC</t>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENKASHRRSAC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">near kateawla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">manager</t>
@@ -154,7 +199,7 @@
     <t xml:space="preserve">SBI Mira Road</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">dsadas</t>
   </si>
   <si>
     <t xml:space="preserve">Tapped</t>
@@ -163,10 +208,28 @@
     <t xml:space="preserve">Manager seems to be friendly</t>
   </si>
   <si>
-    <t xml:space="preserve">Choco Pie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADF</t>
+    <t xml:space="preserve">Choco Pie test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENKASHRRSAD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdsafsd fdsfsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsdas</t>
   </si>
   <si>
     <t xml:space="preserve">LetterGiven</t>
@@ -277,26 +340,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="55.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -393,207 +452,288 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>401105</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="I2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>19.3019896</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="M2" s="1" t="n">
         <v>72.8626008</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="N2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="O2" s="1" t="n">
         <v>918</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="1" t="n">
+      <c r="P2" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="n">
         <v>9090909090</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="W2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>2000302202</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>2121</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AM2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>401105</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>19.3019896</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>72.8626008</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>918</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>9090909090</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" s="1" t="n">
         <v>2000302202</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="1" t="n">
+      <c r="AA3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="AC2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="AD2" s="2" t="n">
+      <c r="AG3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>401105</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>19.3019896</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>72.8626008</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>918</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="1" t="n">
-        <v>9090909090</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>2000302202</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="AC3" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="AD3" s="2" t="n">
+      <c r="AL3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>50</v>
+      <c r="AM3" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
@bugfix - some fix for import society data
</commit_message>
<xml_diff>
--- a/coreapi/coreapi/v0/society_data.xlsx
+++ b/coreapi/coreapi/v0/society_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t xml:space="preserve">Society Name</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landline Number</t>
   </si>
   <si>
     <t xml:space="preserve">Name of Payment</t>
@@ -340,19 +343,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="35" min="31" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,40 +486,43 @@
       <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>401105</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>19.3019896</v>
@@ -530,114 +540,115 @@
         <v>22</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V2" s="1" t="n">
         <v>9090909090</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="Z2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" s="1" t="n">
         <v>2000302202</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB2" s="1" t="n">
+      <c r="AB2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" s="1" t="n">
         <v>2121</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD2" s="1" t="n">
+      <c r="AD2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF2" s="1" t="n">
+      <c r="AF2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH2" s="1" t="n">
+      <c r="AH2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
+      <c r="AJ2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AK2" s="2" t="n">
+      <c r="AL2" s="2" t="n">
         <v>10000</v>
-      </c>
-      <c r="AL2" s="2" t="n">
-        <v>1000</v>
       </c>
       <c r="AM2" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AN2" s="2" t="s">
-        <v>60</v>
+      <c r="AN2" s="2" t="n">
+        <v>1000</v>
       </c>
       <c r="AO2" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="AP2" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="24.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>401105</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>19.3019896</v>
@@ -655,67 +666,65 @@
         <v>22</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>9090909090</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" s="1" t="n">
+      <c r="Z3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="1" t="n">
         <v>2000302202</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB3" s="1" t="n">
+      <c r="AB3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC3" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD3" s="1" t="n">
+      <c r="AD3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AE3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" s="1" t="n">
+      <c r="AF3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AG3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH3" s="1" t="n">
+      <c r="AH3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AI3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ3" s="1" t="n">
+      <c r="AJ3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK3" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="AK3" s="2" t="n">
-        <v>1000</v>
       </c>
       <c r="AL3" s="2" t="n">
         <v>1000</v>
@@ -723,11 +732,14 @@
       <c r="AM3" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="AN3" s="2" t="s">
-        <v>70</v>
+      <c r="AN3" s="2" t="n">
+        <v>1000</v>
       </c>
       <c r="AO3" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>